<commit_message>
tab synthèse à jour
</commit_message>
<xml_diff>
--- a/code/public/Tab_synthèse.xlsx
+++ b/code/public/Tab_synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\portfolio-V2\code\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC6EEE7-4DE4-4E8A-A905-25DC78EC3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DB2D21-F171-4D73-969E-78759D316A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : https://matthieu77220.github.io/portfolio-V2</t>
+  </si>
+  <si>
+    <t>Habitly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          en cours</t>
+  </si>
+  <si>
+    <t>FreelanceHub</t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -726,15 +735,39 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -768,29 +801,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1201,68 +1216,68 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="70.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.44140625" customWidth="1"/>
     <col min="44" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1274,22 +1289,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1312,8 +1327,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="19" t="s">
         <v>16</v>
       </c>
@@ -1369,16 +1384,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1419,7 +1434,9 @@
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="45">
+        <v>45658</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
         <v>23</v>
@@ -1474,7 +1491,9 @@
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="44">
+        <v>45717</v>
+      </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
         <v>23</v>
@@ -1529,7 +1548,9 @@
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="44">
+        <v>45717</v>
+      </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
         <v>23</v>
@@ -1581,14 +1602,28 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
+      <c r="D12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1626,14 +1661,26 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="F13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>23</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1896,16 +1943,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2268,16 +2315,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2722,11 +2769,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2734,6 +2776,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A5">
@@ -2763,14 +2810,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9afeb195-fe8e-4d53-b966-ac86e014f9d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b96438d6-4088-444b-a148-08e2a0c42289" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2975,21 +3020,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9afeb195-fe8e-4d53-b966-ac86e014f9d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b96438d6-4088-444b-a148-08e2a0c42289" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA3166D-F719-49F0-B698-E9057D9EDF6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574C0259-CE3C-4D74-A0FE-24A73702E787}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9afeb195-fe8e-4d53-b966-ac86e014f9d0"/>
-    <ds:schemaRef ds:uri="b96438d6-4088-444b-a148-08e2a0c42289"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3014,9 +3058,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574C0259-CE3C-4D74-A0FE-24A73702E787}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA3166D-F719-49F0-B698-E9057D9EDF6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9afeb195-fe8e-4d53-b966-ac86e014f9d0"/>
+    <ds:schemaRef ds:uri="b96438d6-4088-444b-a148-08e2a0c42289"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>